<commit_message>
Added different folder structure for emails
</commit_message>
<xml_diff>
--- a/SoftwareBot/Email sample Uipath.xlsx
+++ b/SoftwareBot/Email sample Uipath.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\Projekti-2-Ohjelmistorobotti\SoftwareBot\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9699E27-3E94-4C94-AA33-2039BA992FCE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C88EC5EF-FA13-4856-AE14-FD557AEA42C2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15780" yWindow="6075" windowWidth="14595" windowHeight="8925" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="8988" yWindow="3504" windowWidth="23040" windowHeight="12264" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -25,12 +25,6 @@
     <t>eero.oittinen@student.lab.fi</t>
   </si>
   <si>
-    <t>Eero</t>
-  </si>
-  <si>
-    <t>Nimi</t>
-  </si>
-  <si>
     <t>Sähköposti</t>
   </si>
   <si>
@@ -46,10 +40,16 @@
     <t>Testi</t>
   </si>
   <si>
-    <t>Eero2</t>
-  </si>
-  <si>
     <t>eero.oittinen@gmail.com</t>
+  </si>
+  <si>
+    <t>Yrityksen nimi</t>
+  </si>
+  <si>
+    <t>RoboCamp demoyritys 1</t>
+  </si>
+  <si>
+    <t>Ohjelmistorobotti</t>
   </si>
 </sst>
 </file>
@@ -391,56 +391,56 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="C1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D1" t="s">
-        <v>5</v>
-      </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>9</v>
-      </c>
       <c r="C3" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D3" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Yhdistellyt palikat, ei toimi vielä. Kirjoittaa exceliin.
</commit_message>
<xml_diff>
--- a/SoftwareBot/Email sample Uipath.xlsx
+++ b/SoftwareBot/Email sample Uipath.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\Projekti-2-Ohjelmistorobotti\SoftwareBot\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\karit\OneDrive\Tiedostot\Botti\SoftwareBot\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B46DDAA-3CCC-48AD-AA22-6AB9DAC2EF53}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3127D7E-14F3-45E8-BEBB-E8D7D9EB0302}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9375" yWindow="2220" windowWidth="28785" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -20,10 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="22">
-  <si>
-    <t>eero.oittinen@student.lab.fi</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="9">
   <si>
     <t>Sähköposti</t>
   </si>
@@ -40,9 +37,6 @@
     <t>Testi</t>
   </si>
   <si>
-    <t>eero.oittinen@gmail.com</t>
-  </si>
-  <si>
     <t>Yrityksen nimi</t>
   </si>
   <si>
@@ -52,40 +46,7 @@
     <t>Ohjelmistorobotti</t>
   </si>
   <si>
-    <t>testi</t>
-  </si>
-  <si>
-    <t>testi1</t>
-  </si>
-  <si>
-    <t>testi2</t>
-  </si>
-  <si>
-    <t>testi3</t>
-  </si>
-  <si>
-    <t>testi4</t>
-  </si>
-  <si>
-    <t>testi5</t>
-  </si>
-  <si>
-    <t>testi6</t>
-  </si>
-  <si>
-    <t>testi7</t>
-  </si>
-  <si>
-    <t>testi8</t>
-  </si>
-  <si>
-    <t>testi9</t>
-  </si>
-  <si>
-    <t>testi10</t>
-  </si>
-  <si>
-    <t>testi11</t>
+    <t>toni.kari@student.lab.fi</t>
   </si>
 </sst>
 </file>
@@ -424,119 +385,59 @@
     <outlinePr summaryBelow="0" summaryRight="0"/>
     <pageSetUpPr autoPageBreaks="0" fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:D15"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:A15"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>7</v>
       </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
+      <c r="B3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" t="s">
         <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>